<commit_message>
Update the scrum-file for sprint 2
</commit_message>
<xml_diff>
--- a/documentation/Task8-Sprint2/scrum_v02.xlsx
+++ b/documentation/Task8-Sprint2/scrum_v02.xlsx
@@ -1,32 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yaron\OneDrive\SoED CS2\Task 6\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TempUserProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_1212\AC\Temp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="11_4E29E552DF7DEE361965C1565A9BF00D45272AFB" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{47F85EB2-861C-412F-B727-3D6F9F320987}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="11_4E29E552DF7DEE361965C1565A9BF00D45272AFB" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{B137BA1E-5FB3-4801-9815-EB70F42327C8}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="753" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" tabRatio="753" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
     <sheet name="Product Backlog" sheetId="1" r:id="rId2"/>
     <sheet name="Status overview" sheetId="5" r:id="rId3"/>
-    <sheet name="Sprint Backlog" sheetId="2" r:id="rId4"/>
-    <sheet name="BurndownChart" sheetId="4" r:id="rId5"/>
+    <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint Backlog" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Sprint Backlog'!$A$1:$L$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Sprint Backlog'!$A$1:$L$29</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -72,6 +73,9 @@
     <t>oppli</t>
   </si>
   <si>
+    <t>Team</t>
+  </si>
+  <si>
     <t>ID</t>
   </si>
   <si>
@@ -258,6 +262,18 @@
     <t>Der Task wird nicht umgesetzt.</t>
   </si>
   <si>
+    <t xml:space="preserve">Sprint </t>
+  </si>
+  <si>
+    <t>Time of Record</t>
+  </si>
+  <si>
+    <t>Remaining Effort</t>
+  </si>
+  <si>
+    <t>Remaining Ressources</t>
+  </si>
+  <si>
     <t>Sprint</t>
   </si>
   <si>
@@ -307,6 +323,9 @@
   </si>
   <si>
     <t>SeminarManager SeminarPresenter</t>
+  </si>
+  <si>
+    <t>Fertig aber nicht gemerged.</t>
   </si>
   <si>
     <t>neues Seminar erfassen Maske erstellen</t>
@@ -406,9 +425,21 @@
     <t>Seminar: Standort auf Karte anzeigen</t>
   </si>
   <si>
+    <t>Einfügen von einer Google-Map Karte, und auf dieser dann die Seminare anzeigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SeminarView </t>
+  </si>
+  <si>
     <t>Seminar: Daten abspeichern</t>
   </si>
   <si>
+    <t>Die Seminare sollen in der angehängten DB gespeichert werden können.</t>
+  </si>
+  <si>
+    <t>SeminarRepository, SeminarManager</t>
+  </si>
+  <si>
     <t>Home-Page: Hot Topics</t>
   </si>
   <si>
@@ -418,37 +449,46 @@
     <t>User abspeichern</t>
   </si>
   <si>
+    <t xml:space="preserve">Die User sollen in der DB gespeichert werden. </t>
+  </si>
+  <si>
+    <t>UserManager, UserRepository</t>
+  </si>
+  <si>
     <t>Berechtigunskonzept umsetzen</t>
   </si>
   <si>
+    <t>Session-User auslesen, sowie beim an- und abmelden jeweils den Session-User anpassen. In den Manager-Klassen jeweils noch zusätzlich überprüfen, ob der User das notwendige Recht für die Aktion hat.</t>
+  </si>
+  <si>
+    <t>UserManager, SeminarView, NewSeminarView</t>
+  </si>
+  <si>
     <t>Datenbankanbindung</t>
   </si>
   <si>
-    <t xml:space="preserve">Sprint </t>
-  </si>
-  <si>
-    <t>Time of Record</t>
-  </si>
-  <si>
-    <t>Remaining Effort</t>
-  </si>
-  <si>
-    <t>Remaining Ressources</t>
-  </si>
-  <si>
-    <t>Einfügen von einer Google-Map Karte, und auf dieser dann die Seminare anzeigen</t>
+    <t>H2 anbinden, die Mock-Daten in SQL umwandeln, damit diese jeweils beim Start der Applikation geladen werden können</t>
+  </si>
+  <si>
+    <t>Repository-Klassen, Spring, H2</t>
   </si>
   <si>
     <t>Layout erstellen</t>
   </si>
   <si>
-    <t>Session-User auslesen, sowie beim an- und abmelden jeweils den Session-User anpassen. In den Manager-Klassen jeweils noch zusätzlich überprüfen, ob der User das notwendige Recht für die Aktion hat.</t>
-  </si>
-  <si>
     <t>Unser aktuelles Layout nimmt 1/3 der Breite ein und ist dennoch zu breit (scrollbar horizontal), die Webapplikation etwas aufhübschen, damit nicht alles einfach weiss ist.</t>
   </si>
   <si>
-    <t>H2 anbinden, die Mock-Daten in SQL umwandeln, damit diese jeweils beim Start der Applikation geladen werden können</t>
+    <t>SeminarView, HomeView</t>
+  </si>
+  <si>
+    <t>Passwortspeicherung verbessern</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zurzeit wird das Passwort im Plain-Text gespeichert. Das soll geändert werden. </t>
+  </si>
+  <si>
+    <t>UserManager, User</t>
   </si>
   <si>
     <t>Seminar-GUI überarbeiten</t>
@@ -457,34 +497,25 @@
     <t>MVP umsetzen, Filter zurücksetzen, Enter-Taste implementieren, klarere Anzeige der Verfügbarkeit von Details (z.B. Info-Logo).</t>
   </si>
   <si>
-    <t>Fertig aber nicht gemerged.</t>
-  </si>
-  <si>
     <t xml:space="preserve">MVP umsetzen für Konstanten, Mergen. </t>
   </si>
   <si>
+    <t>Seminar: Neues Seminar - Maske anpassen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Elemente in der Maske nach Spring-Update korrigieren. MVP verbessern, Fehlermeldungen in der Ecke oben, Route anpassen. </t>
   </si>
   <si>
-    <t>Seminar: Neues Seminar - Maske anpassen</t>
+    <t>Seminare: Filter anpassen</t>
   </si>
   <si>
     <t>Keyword-Filtering anpassen. (Nicht oder sondern und) (Nur nach Titel oder Description filtern.) MVP anpassen (View muss Presenter aufrufen für Update)</t>
   </si>
   <si>
-    <t>Seminare: Filter anpassen</t>
-  </si>
-  <si>
     <t>MVP verbessern</t>
   </si>
   <si>
-    <t>Die Seminare sollen in der angehängten DB gespeichert werden können.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Die User sollen in der DB gespeichert werden. </t>
-  </si>
-  <si>
-    <t>SeminarView, HomeView</t>
+    <t>HomeLayout MainView </t>
   </si>
   <si>
     <t>Class Diagram and Persistence</t>
@@ -493,44 +524,14 @@
     <t xml:space="preserve">Die neue Modul-Aufgabe muss gelöst werden. Die Repository-Inerfaces bestehen bereits, aufgrund von Spring wird keine Implementation benötigt, ausser im Falle komplexer Querys. </t>
   </si>
   <si>
-    <t>HomeLayout MainView </t>
-  </si>
-  <si>
-    <t>Team</t>
-  </si>
-  <si>
     <t>Dokument auf GIT</t>
-  </si>
-  <si>
-    <t>Passwortspeicherung verbessern</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Zurzeit wird das Passwort im Plain-Text gespeichert. Das soll geändert werden. </t>
-  </si>
-  <si>
-    <t>UserManager, User</t>
-  </si>
-  <si>
-    <t>Repository-Klassen, Spring, H2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SeminarView </t>
-  </si>
-  <si>
-    <t>SeminarRepository, SeminarManager</t>
-  </si>
-  <si>
-    <t>UserManager, UserRepository</t>
-  </si>
-  <si>
-    <t>UserManager, SeminarView, NewSeminarView</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -640,7 +641,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -966,13 +967,13 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="18.7265625" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="19.350000000000001" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -980,7 +981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="15">
       <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
@@ -988,7 +989,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="15">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -996,7 +997,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="15">
       <c r="A5" s="6" t="s">
         <v>8</v>
       </c>
@@ -1012,7 +1013,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="15">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
@@ -1020,9 +1021,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="15">
       <c r="A7" s="6" t="s">
-        <v>153</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1038,76 +1039,76 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="3.81640625" customWidth="1"/>
-    <col min="2" max="2" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.1796875" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" customWidth="1"/>
-    <col min="5" max="5" width="11.54296875" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" customWidth="1"/>
-    <col min="7" max="7" width="10.1796875" customWidth="1"/>
-    <col min="8" max="8" width="14.453125" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" s="3" customFormat="1" ht="30">
       <c r="A1" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="58" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="60">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" s="1">
         <v>12</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E3" s="1">
         <v>10</v>
@@ -1115,7 +1116,7 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -1128,18 +1129,18 @@
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1">
         <v>5</v>
@@ -1147,7 +1148,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -1160,18 +1161,18 @@
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:18" ht="45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1">
         <v>6</v>
@@ -1179,7 +1180,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1192,18 +1193,18 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" ht="45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1">
         <v>10</v>
@@ -1211,7 +1212,7 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -1224,18 +1225,18 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" ht="75">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="E7" s="1">
         <v>15</v>
@@ -1243,7 +1244,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1256,18 +1257,18 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" ht="75">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1">
         <v>8</v>
@@ -1275,7 +1276,7 @@
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1288,18 +1289,18 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" ht="60">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E9" s="1">
         <v>15</v>
@@ -1307,7 +1308,7 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
       <c r="H9" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1320,18 +1321,18 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" ht="75">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E10" s="1">
         <v>8</v>
@@ -1339,7 +1340,7 @@
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -1352,18 +1353,18 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" ht="45">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E11" s="1">
         <v>20</v>
@@ -1371,7 +1372,7 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -1384,18 +1385,18 @@
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" ht="120">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E12" s="1">
         <v>30</v>
@@ -1403,7 +1404,7 @@
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -1416,18 +1417,18 @@
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" ht="75">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E13" s="1">
         <v>6</v>
@@ -1435,7 +1436,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -1448,18 +1449,18 @@
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="58" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" ht="60">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E14" s="1">
         <v>6</v>
@@ -1467,7 +1468,7 @@
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1480,18 +1481,18 @@
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" ht="30">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E15" s="1">
         <v>7</v>
@@ -1499,7 +1500,7 @@
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -1512,18 +1513,18 @@
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" ht="75">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1">
         <v>3</v>
@@ -1531,7 +1532,7 @@
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -1544,18 +1545,18 @@
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" ht="101.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" ht="105">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E17" s="1">
         <v>9</v>
@@ -1563,7 +1564,7 @@
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1576,18 +1577,18 @@
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="30">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E18" s="1">
         <v>5</v>
@@ -1595,7 +1596,7 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -1608,18 +1609,18 @@
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" ht="72.599999999999994" customHeight="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E19" s="1">
         <v>8</v>
@@ -1627,7 +1628,7 @@
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1640,7 +1641,7 @@
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:18" ht="15">
       <c r="E32">
         <f>SUM(E2:E19)</f>
         <v>183</v>
@@ -1660,73 +1661,73 @@
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="14.45"/>
   <cols>
-    <col min="2" max="2" width="110.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="110.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15">
       <c r="A4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15">
       <c r="A7" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1735,73 +1736,138 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
+  <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="4" customFormat="1" ht="26.45" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>42262</v>
+      </c>
+      <c r="C2">
+        <v>45</v>
+      </c>
+      <c r="D2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5">
+        <v>42263</v>
+      </c>
+      <c r="C3">
+        <f>C2-5</f>
+        <v>40</v>
+      </c>
+      <c r="D3">
+        <f>D2-5</f>
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="D27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L28" sqref="L28"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="6.1796875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="34.54296875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="9" customWidth="1"/>
     <col min="4" max="4" width="44" style="9" customWidth="1"/>
-    <col min="5" max="5" width="22.1796875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" style="9" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="7.81640625" style="9" customWidth="1"/>
-    <col min="10" max="10" width="9.1796875" style="9" customWidth="1"/>
-    <col min="11" max="11" width="7.1796875" style="9" customWidth="1"/>
-    <col min="12" max="12" width="15.1796875" style="9" customWidth="1"/>
-    <col min="13" max="13" width="60.453125" style="9" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="9"/>
+    <col min="5" max="5" width="22.140625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="9" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="9" customWidth="1"/>
+    <col min="12" max="12" width="15.140625" style="9" customWidth="1"/>
+    <col min="13" max="13" width="60.42578125" style="9" customWidth="1"/>
+    <col min="14" max="16384" width="8.7109375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="11" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="11" customFormat="1" ht="60">
       <c r="A1" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="L1" s="11" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="58" hidden="1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="75" hidden="1">
       <c r="A2" s="8">
         <v>1.1000000000000001</v>
       </c>
@@ -1809,22 +1875,22 @@
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I2" s="8">
         <v>2</v>
@@ -1834,11 +1900,11 @@
         <v>1</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M2" s="8"/>
     </row>
-    <row r="3" spans="1:13" ht="72.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" ht="75" hidden="1">
       <c r="A3" s="8">
         <v>1.2</v>
       </c>
@@ -1846,22 +1912,22 @@
         <v>1</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I3" s="8">
         <v>6</v>
@@ -1871,11 +1937,11 @@
         <v>6</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M3" s="8"/>
     </row>
-    <row r="4" spans="1:13" ht="101.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="120" hidden="1">
       <c r="A4" s="8">
         <v>2.1</v>
       </c>
@@ -1883,22 +1949,22 @@
         <v>1</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I4" s="8">
         <v>4</v>
@@ -1908,13 +1974,13 @@
         <v>4.5</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="58" hidden="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="60" hidden="1">
       <c r="A5" s="8">
         <v>2.2000000000000002</v>
       </c>
@@ -1922,22 +1988,22 @@
         <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I5" s="8">
         <v>6</v>
@@ -1947,11 +2013,11 @@
         <v>9</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M5" s="8"/>
     </row>
-    <row r="6" spans="1:13" ht="87.75" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="87.75" hidden="1" customHeight="1">
       <c r="A6" s="8">
         <v>4.0999999999999996</v>
       </c>
@@ -1959,22 +2025,22 @@
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I6" s="8">
         <v>1</v>
@@ -1984,11 +2050,11 @@
         <v>5</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M6" s="8"/>
     </row>
-    <row r="7" spans="1:13" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="60" hidden="1">
       <c r="A7" s="8">
         <v>4.2</v>
       </c>
@@ -1996,22 +2062,22 @@
         <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I7" s="8">
         <v>5</v>
@@ -2021,11 +2087,11 @@
         <v>3</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="45" hidden="1">
       <c r="A8" s="8">
         <v>16.100000000000001</v>
       </c>
@@ -2033,22 +2099,22 @@
         <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I8" s="8">
         <v>3</v>
@@ -2058,11 +2124,11 @@
         <v>4</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M8" s="8"/>
     </row>
-    <row r="9" spans="1:13" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="60" hidden="1">
       <c r="A9" s="8">
         <v>16.2</v>
       </c>
@@ -2070,22 +2136,22 @@
         <v>1</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I9" s="8">
         <v>4</v>
@@ -2095,11 +2161,11 @@
         <v>3</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M9" s="8"/>
     </row>
-    <row r="10" spans="1:13" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="45" hidden="1">
       <c r="A10" s="8">
         <v>16.3</v>
       </c>
@@ -2107,22 +2173,22 @@
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I10" s="8">
         <v>2</v>
@@ -2132,11 +2198,11 @@
         <v>2</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M10" s="8"/>
     </row>
-    <row r="11" spans="1:13" ht="87" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="105" hidden="1">
       <c r="A11" s="8">
         <v>17.100000000000001</v>
       </c>
@@ -2144,22 +2210,22 @@
         <v>1</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I11" s="8">
         <v>2</v>
@@ -2169,11 +2235,11 @@
         <v>2</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M11" s="8"/>
     </row>
-    <row r="12" spans="1:13" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="75" hidden="1">
       <c r="A12" s="8">
         <v>17.3</v>
       </c>
@@ -2181,22 +2247,22 @@
         <v>1</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>113</v>
+        <v>119</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I12" s="8">
         <v>1</v>
@@ -2205,11 +2271,11 @@
         <v>0.5</v>
       </c>
       <c r="L12" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M12" s="8"/>
     </row>
-    <row r="13" spans="1:13" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="60" hidden="1">
       <c r="A13" s="8">
         <v>0.1</v>
       </c>
@@ -2217,22 +2283,22 @@
         <v>1</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I13" s="8">
         <v>3</v>
@@ -2242,11 +2308,11 @@
         <v>2</v>
       </c>
       <c r="L13" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M13" s="8"/>
     </row>
-    <row r="14" spans="1:13" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="45" hidden="1">
       <c r="A14" s="8">
         <v>0.2</v>
       </c>
@@ -2254,22 +2320,22 @@
         <v>1</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>116</v>
+        <v>122</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I14" s="8">
         <v>6</v>
@@ -2279,11 +2345,11 @@
         <v>8</v>
       </c>
       <c r="L14" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M14" s="8"/>
     </row>
-    <row r="15" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="45">
       <c r="A15" s="8">
         <v>3.2</v>
       </c>
@@ -2291,33 +2357,35 @@
         <v>2</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>120</v>
+        <v>126</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I15" s="8">
         <v>1</v>
       </c>
       <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="K15" s="8">
+        <v>0.5</v>
+      </c>
       <c r="L15" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="29" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="30">
       <c r="A16" s="8">
         <v>1.3</v>
       </c>
@@ -2325,33 +2393,37 @@
         <v>2</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>159</v>
+        <v>130</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I16" s="8">
         <v>6</v>
       </c>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="J16" s="8">
+        <v>9</v>
+      </c>
+      <c r="K16" s="8">
+        <v>6</v>
+      </c>
       <c r="L16" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="30">
       <c r="A17" s="8">
         <v>2.2999999999999998</v>
       </c>
@@ -2359,50 +2431,52 @@
         <v>2</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>160</v>
+        <v>133</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I17" s="8">
         <v>1</v>
       </c>
       <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
+      <c r="K17" s="8">
+        <v>1.5</v>
+      </c>
       <c r="L17" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" ht="29" hidden="1" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="30" hidden="1">
       <c r="A18" s="8">
         <v>16.399999999999999</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H18" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="I18" s="8">
         <v>2</v>
@@ -2410,10 +2484,10 @@
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
       <c r="L18" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="30">
       <c r="A19" s="8">
         <v>17.2</v>
       </c>
@@ -2421,33 +2495,35 @@
         <v>2</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I19" s="8">
         <v>1</v>
       </c>
       <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
+      <c r="K19" s="8">
+        <v>2</v>
+      </c>
       <c r="L19" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" ht="72.5" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="75">
       <c r="A20" s="8">
         <v>18.100000000000001</v>
       </c>
@@ -2455,33 +2531,35 @@
         <v>2</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I20" s="8">
         <v>8</v>
       </c>
       <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
+      <c r="K20" s="8">
+        <v>6</v>
+      </c>
       <c r="L20" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="45">
       <c r="A21" s="8">
         <v>0.3</v>
       </c>
@@ -2489,56 +2567,58 @@
         <v>2</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>128</v>
+        <v>142</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>2</v>
       </c>
       <c r="G21" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H21" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I21" s="8">
         <v>9</v>
       </c>
       <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
+      <c r="K21" s="8">
+        <v>9</v>
+      </c>
       <c r="L21" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="75" hidden="1">
       <c r="A22" s="8">
         <v>0.4</v>
       </c>
       <c r="B22" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>134</v>
+        <v>145</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I22" s="8">
         <v>6</v>
@@ -2546,12 +2626,12 @@
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
       <c r="L22" s="8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:14" ht="30">
       <c r="A23" s="8">
         <v>17.3</v>
       </c>
@@ -2559,35 +2639,37 @@
         <v>2</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="F23" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I23" s="8">
         <v>2.5</v>
       </c>
       <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
+      <c r="K23" s="8">
+        <v>4.5</v>
+      </c>
       <c r="L23" s="8" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:14" ht="45">
       <c r="A24" s="8">
         <v>1.2</v>
       </c>
@@ -2595,35 +2677,37 @@
         <v>2</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>10</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I24" s="8">
         <v>4</v>
       </c>
       <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
+      <c r="K24" s="8">
+        <v>4</v>
+      </c>
       <c r="L24" s="8" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:14" ht="30">
       <c r="A25" s="8">
         <v>2.1</v>
       </c>
@@ -2631,35 +2715,37 @@
         <v>2</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="F25" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I25" s="8">
         <v>2</v>
       </c>
       <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
+      <c r="K25" s="8">
+        <v>1</v>
+      </c>
       <c r="L25" s="10" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="M25" s="8"/>
       <c r="N25" s="8"/>
     </row>
-    <row r="26" spans="1:14" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:14" ht="60">
       <c r="A26" s="8">
         <v>2.2000000000000002</v>
       </c>
@@ -2667,34 +2753,36 @@
         <v>2</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="F26" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I26" s="8">
         <v>3</v>
       </c>
       <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
+      <c r="K26" s="8">
+        <v>3</v>
+      </c>
       <c r="L26" s="10" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="M26" s="8"/>
     </row>
-    <row r="27" spans="1:14" ht="87.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:14" ht="87.75" customHeight="1">
       <c r="A27" s="8">
         <v>4.0999999999999996</v>
       </c>
@@ -2702,34 +2790,36 @@
         <v>2</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>8</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I27" s="8">
         <v>2.5</v>
       </c>
       <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
+      <c r="K27" s="8">
+        <v>1</v>
+      </c>
       <c r="L27" s="10" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="M27" s="8"/>
     </row>
-    <row r="28" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:14" ht="45">
       <c r="A28" s="8">
         <v>16.100000000000001</v>
       </c>
@@ -2737,34 +2827,36 @@
         <v>2</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="F28" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G28" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H28" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I28" s="8">
         <v>1</v>
       </c>
       <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
+      <c r="K28" s="8">
+        <v>3</v>
+      </c>
       <c r="L28" s="10" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="M28" s="8"/>
     </row>
-    <row r="29" spans="1:14" ht="58" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:14" ht="75">
       <c r="A29" s="8">
         <v>0.5</v>
       </c>
@@ -2772,35 +2864,39 @@
         <v>2</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>153</v>
+        <v>10</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="H29" s="8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I29" s="8">
         <v>1</v>
       </c>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="J29" s="8">
+        <v>6</v>
+      </c>
+      <c r="K29" s="8">
+        <v>6</v>
+      </c>
       <c r="L29" s="8" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="M29" s="8"/>
       <c r="N29" s="8"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:14" ht="15">
       <c r="A30" s="8"/>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -2816,7 +2912,7 @@
       <c r="M30" s="8"/>
       <c r="N30" s="8"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" ht="15">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -2832,7 +2928,7 @@
       <c r="M31" s="8"/>
       <c r="N31" s="8"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:14" ht="15">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -2848,7 +2944,7 @@
       <c r="M32" s="8"/>
       <c r="N32" s="8"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:14" ht="15">
       <c r="A33" s="8"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -2864,7 +2960,7 @@
       <c r="M33" s="8"/>
       <c r="N33" s="8"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:14" ht="15">
       <c r="A34" s="8"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -2880,7 +2976,7 @@
       <c r="M34" s="8"/>
       <c r="N34" s="8"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:14" ht="15">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -2896,7 +2992,7 @@
       <c r="M35" s="8"/>
       <c r="N35" s="8"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:14" ht="15">
       <c r="A36" s="8"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -2912,7 +3008,7 @@
       <c r="M36" s="8"/>
       <c r="N36" s="8"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:14" ht="15">
       <c r="A37" s="8"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -2928,7 +3024,7 @@
       <c r="M37" s="8"/>
       <c r="N37" s="8"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:14" ht="15">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -2944,7 +3040,7 @@
       <c r="M38" s="8"/>
       <c r="N38" s="8"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:14" ht="15">
       <c r="A39" s="8"/>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
@@ -2960,7 +3056,7 @@
       <c r="M39" s="8"/>
       <c r="N39" s="8"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:14" ht="15">
       <c r="A40" s="8"/>
       <c r="B40" s="8"/>
       <c r="C40" s="8"/>
@@ -2976,7 +3072,7 @@
       <c r="M40" s="8"/>
       <c r="N40" s="8"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:14" ht="15">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -2992,7 +3088,7 @@
       <c r="M41" s="8"/>
       <c r="N41" s="8"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:14" ht="15">
       <c r="A42" s="8"/>
       <c r="B42" s="8"/>
       <c r="C42" s="8"/>
@@ -3008,7 +3104,7 @@
       <c r="M42" s="8"/>
       <c r="N42" s="8"/>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:14" ht="15">
       <c r="A43" s="8"/>
       <c r="B43" s="8"/>
       <c r="C43" s="8"/>
@@ -3024,7 +3120,7 @@
       <c r="M43" s="8"/>
       <c r="N43" s="8"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:14" ht="15">
       <c r="A44" s="8"/>
       <c r="B44" s="8"/>
       <c r="C44" s="8"/>
@@ -3040,7 +3136,7 @@
       <c r="M44" s="8"/>
       <c r="N44" s="8"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:14" ht="15">
       <c r="A45" s="8"/>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
@@ -3056,7 +3152,7 @@
       <c r="M45" s="8"/>
       <c r="N45" s="8"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:14" ht="15">
       <c r="A46" s="8"/>
       <c r="B46" s="8"/>
       <c r="C46" s="8"/>
@@ -3072,7 +3168,7 @@
       <c r="M46" s="8"/>
       <c r="N46" s="8"/>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:14" ht="15">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="8"/>
@@ -3088,7 +3184,7 @@
       <c r="M47" s="8"/>
       <c r="N47" s="8"/>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:14" ht="15">
       <c r="A48" s="8"/>
       <c r="B48" s="8"/>
       <c r="C48" s="8"/>
@@ -3138,69 +3234,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="4" customFormat="1" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="5">
-        <v>42262</v>
-      </c>
-      <c r="C2">
-        <v>45</v>
-      </c>
-      <c r="D2">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5">
-        <v>42263</v>
-      </c>
-      <c r="C3">
-        <f>C2-5</f>
-        <v>40</v>
-      </c>
-      <c r="D3">
-        <f>D2-5</f>
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>